<commit_message>
Fixed errors in fish order data and regression code
</commit_message>
<xml_diff>
--- a/data/fish_order_family.xlsx
+++ b/data/fish_order_family.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MorganHumphrey/Documents/University/4th Year/Semester 7/IBIO4100/biod-capstone-2024/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MorganHumphrey/Documents/University/4th Year/Semester 7/IBIO4100/mill-creek/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{929FF657-8828-A84C-8472-B0C764CC92C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB97FFC-AA82-334F-9A19-D8D4AF7AB8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{B27DB187-0627-0441-9889-BA9163E59765}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19640" xr2:uid="{B27DB187-0627-0441-9889-BA9163E59765}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="91">
   <si>
     <t>Actinopterygii</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>Catostomidae</t>
-  </si>
-  <si>
-    <t>Scorpaeniformed</t>
   </si>
   <si>
     <t>Cottidae</t>
@@ -715,6 +712,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
@@ -741,7 +739,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
@@ -843,10 +841,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
         <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -860,10 +858,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
         <v>81</v>
-      </c>
-      <c r="C9" t="s">
-        <v>82</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
@@ -894,10 +892,10 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
         <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -914,7 +912,7 @@
         <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
@@ -931,7 +929,7 @@
         <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
@@ -948,7 +946,7 @@
         <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>25</v>
@@ -979,7 +977,7 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
         <v>72</v>
@@ -996,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
         <v>72</v>
@@ -1013,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
@@ -1030,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -1064,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
         <v>72</v>
@@ -1081,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
         <v>72</v>
@@ -1098,10 +1096,10 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>43</v>
@@ -1115,10 +1113,10 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>45</v>
@@ -1135,7 +1133,7 @@
         <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>47</v>
@@ -1217,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>57</v>
@@ -1234,10 +1232,10 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>59</v>
@@ -1254,7 +1252,7 @@
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>61</v>
@@ -1285,10 +1283,10 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>65</v>

</xml_diff>